<commit_message>
Functional, but unstyled window and coding standards added
</commit_message>
<xml_diff>
--- a/Admin and Documentation/DataAll.xlsx
+++ b/Admin and Documentation/DataAll.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="223">
   <si>
     <t>Variable Name</t>
   </si>
@@ -549,12 +549,6 @@
     <t>Pet Age</t>
   </si>
   <si>
-    <t>Ditto</t>
-  </si>
-  <si>
-    <t>Should connect select boxes for 1 choice. One should be required? Radio Button?</t>
-  </si>
-  <si>
     <t>ReferedBy</t>
   </si>
   <si>
@@ -577,6 +571,129 @@
   </si>
   <si>
     <t>Multiple pets based of number of rows</t>
+  </si>
+  <si>
+    <t>Is this in a table? Should it be tracked?</t>
+  </si>
+  <si>
+    <t>Is this in a table? Should be tracked? Just recorded on PDF?</t>
+  </si>
+  <si>
+    <t>Is this in a table? Should it be tracked? Just recorded on PDF?</t>
+  </si>
+  <si>
+    <t>PetNameN etc</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>GpsPrice</t>
+  </si>
+  <si>
+    <t>BPPrice</t>
+  </si>
+  <si>
+    <t>DTPrice</t>
+  </si>
+  <si>
+    <t>OSQuantity</t>
+  </si>
+  <si>
+    <t>OSPrice</t>
+  </si>
+  <si>
+    <t>ISQuantity</t>
+  </si>
+  <si>
+    <t>Currently checkbox</t>
+  </si>
+  <si>
+    <t>Currently checkbox. Should connect select boxes for 1 choice. One should be required? Radio Button? Ever add a pet with nothing entered here?</t>
+  </si>
+  <si>
+    <t>Parts.Quantity</t>
+  </si>
+  <si>
+    <t>OrderDetails.Quantity</t>
+  </si>
+  <si>
+    <t>Needed</t>
+  </si>
+  <si>
+    <t>Out to CRM</t>
+  </si>
+  <si>
+    <t>In and out CRM</t>
+  </si>
+  <si>
+    <t>Need list of part numbers to pull data. In and out to CRM</t>
+  </si>
+  <si>
+    <t>Same as GPS</t>
+  </si>
+  <si>
+    <t>Currently Checkbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In: Parts.PartNumber = ?   &amp;  ADUSERName to get Employee.DealerID Out:Customer.ID, Order.ID, OrderDetail.PartID=? </t>
+  </si>
+  <si>
+    <t>Is This just a subtotal or extra place to add stuff? Can't track item purchased from here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Out:Customer.ID, Order.ID, OrderDetail.PartID=? </t>
+  </si>
+  <si>
+    <t>Parts.PartNumber?</t>
+  </si>
+  <si>
+    <t>Internal number to tabulate Orders.OrderTotal  and Orders TaxableSubtotal</t>
+  </si>
+  <si>
+    <t>Out: Orders.OrdersTotal</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>TaxRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Out: Orders.TaxRate  </t>
+  </si>
+  <si>
+    <t>Orders.TaxTotal</t>
+  </si>
+  <si>
+    <t>SolutionTotal</t>
+  </si>
+  <si>
+    <t>SolutionTotal * TaxRate</t>
+  </si>
+  <si>
+    <t>Where does this feed back into CRM or goes in another way and we just send to PDF?</t>
+  </si>
+  <si>
+    <t>Out: Customer.ID, Order.ID, OrderDetail.PartID = ?</t>
+  </si>
+  <si>
+    <t>Is this saved anywhere or just PDF?</t>
+  </si>
+  <si>
+    <t>Out: OrderDetails.Price</t>
+  </si>
+  <si>
+    <t>In: Parts. Price                  Out:OrderDetails.Price</t>
+  </si>
+  <si>
+    <t>Checkbox to change visibility of coupon textboxes</t>
+  </si>
+  <si>
+    <t>Checkbox to change visibility of discount textboxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -790,7 +907,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -858,35 +975,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -901,6 +989,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3699,1231 +3829,1452 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E190"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" style="42" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="46" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="46" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="40" t="s">
+      <c r="D1" s="36" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="41"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="41"/>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="E3" s="30"/>
+    </row>
+    <row r="4" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="30"/>
+    </row>
+    <row r="6" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="30"/>
+    </row>
+    <row r="7" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="30"/>
+    </row>
+    <row r="8" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="30"/>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="30"/>
+    </row>
+    <row r="10" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C10" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="30"/>
+    </row>
+    <row r="11" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="30"/>
+    </row>
+    <row r="12" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D12" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="41"/>
-    </row>
-    <row r="5" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="41"/>
-    </row>
-    <row r="6" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="41"/>
-    </row>
-    <row r="7" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="41"/>
-    </row>
-    <row r="8" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" s="41"/>
-    </row>
-    <row r="9" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="41"/>
-    </row>
-    <row r="10" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="14" t="s">
+      <c r="E12" s="30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="30"/>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="41"/>
-    </row>
-    <row r="11" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" s="41"/>
-    </row>
-    <row r="12" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="14" t="s">
+      <c r="B15" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="C12" s="14" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D17" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="41"/>
-    </row>
-    <row r="13" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="14" t="s">
+      <c r="E17" s="30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="40"/>
+      <c r="C18" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D18" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="41"/>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="41"/>
-    </row>
-    <row r="15" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="E18" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" s="41"/>
-    </row>
-    <row r="16" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="B16" s="14" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="40"/>
+      <c r="C19" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="40"/>
+      <c r="C20" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="40"/>
+      <c r="C21" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="40"/>
+      <c r="C26" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E30" s="30"/>
+    </row>
+    <row r="31" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="40"/>
+      <c r="C31" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E31" s="30"/>
+    </row>
+    <row r="32" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="40"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="30"/>
+    </row>
+    <row r="33" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E33" s="30"/>
+    </row>
+    <row r="34" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="40"/>
+      <c r="C34" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E34" s="30"/>
+    </row>
+    <row r="35" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="40"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="30"/>
+    </row>
+    <row r="36" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="40"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E36" s="30"/>
+    </row>
+    <row r="37" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="40"/>
+      <c r="C37" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E37" s="30"/>
+    </row>
+    <row r="38" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="40"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="30"/>
+    </row>
+    <row r="39" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="40"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E39" s="30"/>
+    </row>
+    <row r="40" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="40"/>
+      <c r="C40" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E40" s="30"/>
+    </row>
+    <row r="41" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="40"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="30"/>
+    </row>
+    <row r="42" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="40"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E42" s="30"/>
+    </row>
+    <row r="43" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="40"/>
+      <c r="C43" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E43" s="30"/>
+    </row>
+    <row r="44" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="41"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="40"/>
+      <c r="C47" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14" t="s">
+      <c r="D47" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="E47" s="30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="43"/>
+      <c r="C48" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D48" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E48" s="30"/>
+    </row>
+    <row r="49" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B49" s="43"/>
+      <c r="C49" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E49" s="30"/>
+    </row>
+    <row r="50" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="43"/>
+      <c r="C50" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E50" s="30"/>
+    </row>
+    <row r="51" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" s="43"/>
+      <c r="C51" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D51" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E51" s="30"/>
+    </row>
+    <row r="52" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="43"/>
+      <c r="C52" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="41" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14" t="s">
+      <c r="D52" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="E52" s="30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="43"/>
+      <c r="C53" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="41" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="41" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="41" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="41" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="41"/>
-    </row>
-    <row r="24" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="41"/>
-    </row>
-    <row r="25" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="41"/>
-    </row>
-    <row r="26" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="41"/>
-    </row>
-    <row r="27" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="41"/>
-    </row>
-    <row r="28" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="41"/>
-    </row>
-    <row r="29" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="41"/>
-    </row>
-    <row r="30" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="41"/>
-    </row>
-    <row r="31" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="41"/>
-    </row>
-    <row r="32" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="41"/>
-    </row>
-    <row r="33" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="41"/>
-    </row>
-    <row r="34" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="41"/>
-    </row>
-    <row r="35" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="41"/>
-    </row>
-    <row r="36" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="41"/>
-    </row>
-    <row r="37" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="41"/>
-    </row>
-    <row r="38" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="41"/>
-    </row>
-    <row r="39" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="41"/>
-    </row>
-    <row r="40" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="41"/>
-    </row>
-    <row r="41" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="41"/>
-    </row>
-    <row r="42" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="41"/>
-    </row>
-    <row r="43" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="41"/>
-    </row>
-    <row r="44" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="41" t="s">
+      <c r="D53" s="44" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B48" s="32"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="41"/>
-    </row>
-    <row r="49" spans="1:5" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B49" s="32"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="E49" s="41"/>
-    </row>
-    <row r="50" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="B50" s="32"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="41"/>
-    </row>
-    <row r="51" spans="1:5" ht="42" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="B51" s="33"/>
-      <c r="C51" s="34" t="s">
+      <c r="E53" s="30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="43"/>
+      <c r="C54" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D54" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E54" s="30"/>
+    </row>
+    <row r="55" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B55" s="43"/>
+      <c r="C55" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E55" s="30"/>
+    </row>
+    <row r="56" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" s="43"/>
+      <c r="C56" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D56" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E56" s="30"/>
+    </row>
+    <row r="57" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B57" s="43"/>
+      <c r="C57" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D57" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E57" s="30"/>
+    </row>
+    <row r="58" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="B58" s="43"/>
+      <c r="C58" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E58" s="30"/>
+    </row>
+    <row r="59" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="43"/>
+      <c r="C59" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E59" s="30"/>
+    </row>
+    <row r="60" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="43"/>
+      <c r="C60" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="44"/>
+      <c r="E60" s="30"/>
+    </row>
+    <row r="61" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" s="43"/>
+      <c r="C61" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D61" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E61" s="30"/>
+    </row>
+    <row r="62" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62" s="43"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="30"/>
+    </row>
+    <row r="63" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="B63" s="43"/>
+      <c r="C63" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="D63" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="42" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B64" s="43"/>
+      <c r="C64" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="D64" s="42" t="s">
+        <v>205</v>
+      </c>
+      <c r="E64" s="30"/>
+    </row>
+    <row r="65" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B65" s="43"/>
+      <c r="C65" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="D65" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="B66" s="43"/>
+      <c r="C66" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D66" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B67" s="43"/>
+      <c r="C67" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="D51" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="E51" s="41"/>
-    </row>
-    <row r="52" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B52" s="32"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="41" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="B53" s="32"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="41" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B54" s="32"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="41"/>
-    </row>
-    <row r="55" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B55" s="32"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="41"/>
-    </row>
-    <row r="56" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B56" s="32"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="41"/>
-    </row>
-    <row r="57" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B57" s="32"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="41"/>
-    </row>
-    <row r="58" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B58" s="32"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="41"/>
-    </row>
-    <row r="59" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="B59" s="32"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="41"/>
-    </row>
-    <row r="60" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B60" s="32"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="41"/>
-    </row>
-    <row r="61" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="B61" s="32"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="41"/>
-    </row>
-    <row r="62" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B62" s="32"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="41"/>
-    </row>
-    <row r="63" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="B63" s="32"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="41"/>
-    </row>
-    <row r="64" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="B64" s="32"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="41"/>
-    </row>
-    <row r="65" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B65" s="32"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="41"/>
-    </row>
-    <row r="66" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B66" s="32"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="41"/>
-    </row>
-    <row r="67" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="41"/>
-    </row>
-    <row r="68" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="30" t="s">
+      <c r="D67" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="E67" s="30"/>
+    </row>
+    <row r="68" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="B68" s="32"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="41"/>
-    </row>
-    <row r="69" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="30" t="s">
+      <c r="B68" s="43"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="41"/>
-    </row>
-    <row r="70" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="30" t="s">
+      <c r="B69" s="43"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="B70" s="32"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="41"/>
+      <c r="B70" s="43"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="30" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="71" spans="1:5" s="28" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="31" t="s">
+      <c r="A71" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="B71" s="33"/>
-      <c r="C71" s="34"/>
-      <c r="D71" s="39" t="s">
+      <c r="B71" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="D71" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E71" s="41"/>
+      <c r="E71" s="30"/>
     </row>
     <row r="72" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="31" t="s">
+      <c r="A72" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="B72" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="C72" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="D72" s="44"/>
+      <c r="E72" s="30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="B72" s="33"/>
-      <c r="C72" s="34"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="41" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="28" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="31" t="s">
+      <c r="B73" s="43"/>
+      <c r="C73" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="D73" s="44"/>
+      <c r="E73" s="30" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="28" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="B73" s="33"/>
-      <c r="C73" s="34"/>
-      <c r="D73" s="39" t="s">
+      <c r="B74" s="43"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="31"/>
+      <c r="E74" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="E73" s="41"/>
-    </row>
-    <row r="74" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="31" t="s">
+    </row>
+    <row r="75" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="B74" s="33"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="39" t="s">
+      <c r="B75" s="43"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="E74" s="41"/>
-    </row>
-    <row r="75" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="31" t="s">
+    </row>
+    <row r="76" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="B75" s="33"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="41"/>
-    </row>
-    <row r="76" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="31" t="s">
+      <c r="B76" s="43"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="30"/>
+    </row>
+    <row r="77" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="B76" s="33"/>
-      <c r="C76" s="34"/>
-      <c r="D76" s="39" t="s">
+      <c r="B77" s="43"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="46"/>
+      <c r="E77" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="E76" s="41"/>
-    </row>
-    <row r="77" spans="1:5" s="28" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="31" t="s">
+    </row>
+    <row r="78" spans="1:5" s="28" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="B77" s="33"/>
-      <c r="C77" s="34"/>
-      <c r="D77" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="E77" s="41"/>
-    </row>
-    <row r="78" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="31" t="s">
+      <c r="B78" s="43"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="E78" s="30"/>
+    </row>
+    <row r="79" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="B78" s="33"/>
-      <c r="C78" s="34"/>
-      <c r="D78" s="39" t="s">
+      <c r="B79" s="43"/>
+      <c r="C79" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D79" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="E79" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="E78" s="41"/>
-    </row>
-    <row r="79" spans="1:5" s="28" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="31" t="s">
+    </row>
+    <row r="80" spans="1:5" s="28" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="B79" s="33"/>
-      <c r="C79" s="34"/>
-      <c r="D79" s="39" t="s">
+      <c r="B80" s="43"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="E79" s="41"/>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E80" s="43"/>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="44"/>
+      <c r="E80" s="30"/>
+    </row>
+    <row r="81" spans="5:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E81" s="32"/>
     </row>
     <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="44"/>
+      <c r="E82" s="33"/>
     </row>
     <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="44"/>
+      <c r="E83" s="33"/>
     </row>
     <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="44"/>
+      <c r="E84" s="33"/>
     </row>
     <row r="85" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E85" s="44"/>
+      <c r="E85" s="33"/>
     </row>
     <row r="86" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E86" s="44"/>
+      <c r="E86" s="33"/>
     </row>
     <row r="87" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E87" s="44"/>
+      <c r="E87" s="33"/>
     </row>
     <row r="88" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E88" s="44"/>
+      <c r="E88" s="33"/>
     </row>
     <row r="89" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E89" s="44"/>
+      <c r="E89" s="33"/>
     </row>
     <row r="90" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E90" s="44"/>
+      <c r="E90" s="33"/>
     </row>
     <row r="91" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E91" s="44"/>
+      <c r="E91" s="33"/>
     </row>
     <row r="92" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E92" s="44"/>
+      <c r="E92" s="33"/>
     </row>
     <row r="93" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E93" s="44"/>
+      <c r="E93" s="33"/>
     </row>
     <row r="94" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E94" s="44"/>
+      <c r="E94" s="33"/>
     </row>
     <row r="95" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E95" s="44"/>
+      <c r="E95" s="33"/>
     </row>
     <row r="96" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E96" s="44"/>
+      <c r="E96" s="33"/>
     </row>
     <row r="97" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E97" s="44"/>
+      <c r="E97" s="33"/>
     </row>
     <row r="98" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E98" s="44"/>
+      <c r="E98" s="33"/>
     </row>
     <row r="99" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E99" s="44"/>
+      <c r="E99" s="33"/>
     </row>
     <row r="100" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E100" s="44"/>
+      <c r="E100" s="33"/>
     </row>
     <row r="101" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E101" s="44"/>
+      <c r="E101" s="33"/>
     </row>
     <row r="102" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E102" s="44"/>
+      <c r="E102" s="33"/>
     </row>
     <row r="103" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E103" s="44"/>
+      <c r="E103" s="33"/>
     </row>
     <row r="104" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E104" s="44"/>
+      <c r="E104" s="33"/>
     </row>
     <row r="105" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E105" s="44"/>
+      <c r="E105" s="33"/>
     </row>
     <row r="106" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E106" s="44"/>
+      <c r="E106" s="33"/>
     </row>
     <row r="107" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E107" s="44"/>
+      <c r="E107" s="33"/>
     </row>
     <row r="108" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E108" s="44"/>
+      <c r="E108" s="33"/>
     </row>
     <row r="109" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E109" s="44"/>
+      <c r="E109" s="33"/>
     </row>
     <row r="110" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E110" s="44"/>
+      <c r="E110" s="33"/>
     </row>
     <row r="111" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E111" s="44"/>
+      <c r="E111" s="33"/>
     </row>
     <row r="112" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E112" s="44"/>
+      <c r="E112" s="33"/>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E113" s="44"/>
+      <c r="E113" s="33"/>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E114" s="44"/>
+      <c r="E114" s="33"/>
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E115" s="44"/>
+      <c r="E115" s="33"/>
     </row>
     <row r="116" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E116" s="44"/>
+      <c r="E116" s="33"/>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E117" s="44"/>
+      <c r="E117" s="33"/>
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E118" s="44"/>
+      <c r="E118" s="33"/>
     </row>
     <row r="119" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E119" s="44"/>
+      <c r="E119" s="33"/>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E120" s="44"/>
+      <c r="E120" s="33"/>
     </row>
     <row r="121" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E121" s="44"/>
+      <c r="E121" s="33"/>
     </row>
     <row r="122" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E122" s="44"/>
+      <c r="E122" s="33"/>
     </row>
     <row r="123" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E123" s="44"/>
+      <c r="E123" s="33"/>
     </row>
     <row r="124" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E124" s="44"/>
+      <c r="E124" s="33"/>
     </row>
     <row r="125" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E125" s="44"/>
+      <c r="E125" s="33"/>
     </row>
     <row r="126" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E126" s="44"/>
+      <c r="E126" s="33"/>
     </row>
     <row r="127" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E127" s="44"/>
+      <c r="E127" s="33"/>
     </row>
     <row r="128" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E128" s="44"/>
+      <c r="E128" s="33"/>
     </row>
     <row r="129" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E129" s="44"/>
+      <c r="E129" s="33"/>
     </row>
     <row r="130" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E130" s="44"/>
+      <c r="E130" s="33"/>
     </row>
     <row r="131" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E131" s="44"/>
+      <c r="E131" s="33"/>
     </row>
     <row r="132" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E132" s="44"/>
+      <c r="E132" s="33"/>
     </row>
     <row r="133" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E133" s="44"/>
+      <c r="E133" s="33"/>
     </row>
     <row r="134" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E134" s="44"/>
+      <c r="E134" s="33"/>
     </row>
     <row r="135" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E135" s="44"/>
+      <c r="E135" s="33"/>
     </row>
     <row r="136" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E136" s="44"/>
+      <c r="E136" s="33"/>
     </row>
     <row r="137" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E137" s="44"/>
+      <c r="E137" s="33"/>
     </row>
     <row r="138" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E138" s="44"/>
+      <c r="E138" s="33"/>
     </row>
     <row r="139" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E139" s="44"/>
+      <c r="E139" s="33"/>
     </row>
     <row r="140" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E140" s="44"/>
+      <c r="E140" s="33"/>
     </row>
     <row r="141" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E141" s="44"/>
+      <c r="E141" s="33"/>
     </row>
     <row r="142" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E142" s="44"/>
+      <c r="E142" s="33"/>
     </row>
     <row r="143" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E143" s="44"/>
+      <c r="E143" s="33"/>
     </row>
     <row r="144" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E144" s="44"/>
+      <c r="E144" s="33"/>
     </row>
     <row r="145" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E145" s="44"/>
+      <c r="E145" s="33"/>
     </row>
     <row r="146" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E146" s="44"/>
+      <c r="E146" s="33"/>
     </row>
     <row r="147" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E147" s="44"/>
+      <c r="E147" s="33"/>
     </row>
     <row r="148" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E148" s="44"/>
+      <c r="E148" s="33"/>
     </row>
     <row r="149" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E149" s="44"/>
+      <c r="E149" s="33"/>
     </row>
     <row r="150" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E150" s="44"/>
+      <c r="E150" s="33"/>
     </row>
     <row r="151" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E151" s="44"/>
+      <c r="E151" s="33"/>
     </row>
     <row r="152" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E152" s="44"/>
+      <c r="E152" s="33"/>
     </row>
     <row r="153" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E153" s="44"/>
+      <c r="E153" s="33"/>
     </row>
     <row r="154" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E154" s="44"/>
+      <c r="E154" s="33"/>
     </row>
     <row r="155" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E155" s="44"/>
+      <c r="E155" s="33"/>
     </row>
     <row r="156" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E156" s="44"/>
+      <c r="E156" s="33"/>
     </row>
     <row r="157" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E157" s="44"/>
+      <c r="E157" s="33"/>
     </row>
     <row r="158" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E158" s="44"/>
+      <c r="E158" s="33"/>
     </row>
     <row r="159" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E159" s="44"/>
+      <c r="E159" s="33"/>
     </row>
     <row r="160" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E160" s="44"/>
+      <c r="E160" s="33"/>
     </row>
     <row r="161" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E161" s="44"/>
+      <c r="E161" s="33"/>
     </row>
     <row r="162" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E162" s="44"/>
+      <c r="E162" s="33"/>
     </row>
     <row r="163" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E163" s="44"/>
+      <c r="E163" s="33"/>
     </row>
     <row r="164" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E164" s="44"/>
+      <c r="E164" s="33"/>
     </row>
     <row r="165" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E165" s="44"/>
+      <c r="E165" s="33"/>
     </row>
     <row r="166" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E166" s="44"/>
+      <c r="E166" s="33"/>
     </row>
     <row r="167" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E167" s="44"/>
+      <c r="E167" s="33"/>
     </row>
     <row r="168" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E168" s="44"/>
+      <c r="E168" s="33"/>
     </row>
     <row r="169" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E169" s="44"/>
+      <c r="E169" s="33"/>
     </row>
     <row r="170" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E170" s="44"/>
+      <c r="E170" s="33"/>
     </row>
     <row r="171" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E171" s="44"/>
+      <c r="E171" s="33"/>
     </row>
     <row r="172" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E172" s="44"/>
+      <c r="E172" s="33"/>
     </row>
     <row r="173" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E173" s="44"/>
+      <c r="E173" s="33"/>
     </row>
     <row r="174" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E174" s="44"/>
+      <c r="E174" s="33"/>
     </row>
     <row r="175" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E175" s="44"/>
+      <c r="E175" s="33"/>
     </row>
     <row r="176" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E176" s="44"/>
+      <c r="E176" s="33"/>
     </row>
     <row r="177" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E177" s="44"/>
+      <c r="E177" s="33"/>
     </row>
     <row r="178" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E178" s="44"/>
+      <c r="E178" s="33"/>
     </row>
     <row r="179" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E179" s="44"/>
+      <c r="E179" s="33"/>
     </row>
     <row r="180" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E180" s="44"/>
+      <c r="E180" s="33"/>
     </row>
     <row r="181" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E181" s="44"/>
+      <c r="E181" s="33"/>
     </row>
     <row r="182" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E182" s="44"/>
+      <c r="E182" s="33"/>
     </row>
     <row r="183" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E183" s="44"/>
+      <c r="E183" s="33"/>
     </row>
     <row r="184" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E184" s="44"/>
+      <c r="E184" s="33"/>
     </row>
     <row r="185" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E185" s="44"/>
+      <c r="E185" s="33"/>
     </row>
     <row r="186" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E186" s="44"/>
+      <c r="E186" s="33"/>
     </row>
     <row r="187" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E187" s="44"/>
+      <c r="E187" s="33"/>
     </row>
     <row r="188" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E188" s="44"/>
+      <c r="E188" s="33"/>
     </row>
     <row r="189" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E189" s="44"/>
+      <c r="E189" s="33"/>
     </row>
     <row r="190" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E190" s="44"/>
+      <c r="E190" s="33"/>
+    </row>
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E191" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added extra columns and couple formatting updates for pg 2,3,4,7
</commit_message>
<xml_diff>
--- a/Admin and Documentation/DataAll.xlsx
+++ b/Admin and Documentation/DataAll.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="DataAll" sheetId="1" r:id="rId1"/>
-    <sheet name="DataWeek4" sheetId="2" r:id="rId2"/>
+    <sheet name="DataWeek5" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="241">
   <si>
     <t>Variable Name</t>
   </si>
@@ -531,9 +531,6 @@
     <t>Should these be emailed to legal?</t>
   </si>
   <si>
-    <t>Add A Freedom??? See Comment</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -546,12 +543,6 @@
     <t>Pet Name</t>
   </si>
   <si>
-    <t>Pet Age</t>
-  </si>
-  <si>
-    <t>ReferedBy</t>
-  </si>
-  <si>
     <t>HomePhone</t>
   </si>
   <si>
@@ -567,30 +558,15 @@
     <t xml:space="preserve"> Should we just take in Pet Birthday here or do you want age?</t>
   </si>
   <si>
-    <t>Is this being tracked in CRM?</t>
-  </si>
-  <si>
     <t>Multiple pets based of number of rows</t>
   </si>
   <si>
-    <t>Is this in a table? Should it be tracked?</t>
-  </si>
-  <si>
-    <t>Is this in a table? Should be tracked? Just recorded on PDF?</t>
-  </si>
-  <si>
-    <t>Is this in a table? Should it be tracked? Just recorded on PDF?</t>
-  </si>
-  <si>
     <t>PetNameN etc</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>GpsPrice</t>
-  </si>
-  <si>
     <t>BPPrice</t>
   </si>
   <si>
@@ -606,9 +582,6 @@
     <t>ISQuantity</t>
   </si>
   <si>
-    <t>Currently checkbox</t>
-  </si>
-  <si>
     <t>Currently checkbox. Should connect select boxes for 1 choice. One should be required? Radio Button? Ever add a pet with nothing entered here?</t>
   </si>
   <si>
@@ -621,27 +594,15 @@
     <t>Needed</t>
   </si>
   <si>
-    <t>Out to CRM</t>
-  </si>
-  <si>
-    <t>In and out CRM</t>
-  </si>
-  <si>
     <t>Need list of part numbers to pull data. In and out to CRM</t>
   </si>
   <si>
     <t>Same as GPS</t>
   </si>
   <si>
-    <t>Currently Checkbox</t>
-  </si>
-  <si>
     <t xml:space="preserve">In: Parts.PartNumber = ?   &amp;  ADUSERName to get Employee.DealerID Out:Customer.ID, Order.ID, OrderDetail.PartID=? </t>
   </si>
   <si>
-    <t>Is This just a subtotal or extra place to add stuff? Can't track item purchased from here</t>
-  </si>
-  <si>
     <t xml:space="preserve">Out:Customer.ID, Order.ID, OrderDetail.PartID=? </t>
   </si>
   <si>
@@ -678,9 +639,6 @@
     <t>Out: Customer.ID, Order.ID, OrderDetail.PartID = ?</t>
   </si>
   <si>
-    <t>Is this saved anywhere or just PDF?</t>
-  </si>
-  <si>
     <t>Out: OrderDetails.Price</t>
   </si>
   <si>
@@ -693,7 +651,103 @@
     <t>Checkbox to change visibility of discount textboxes</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
+    <t>ReferredBy</t>
+  </si>
+  <si>
+    <t>CustomerNote.NoteTypeID='28'</t>
+  </si>
+  <si>
+    <t>CustomerNote.NoteTypeID = '28'</t>
+  </si>
+  <si>
+    <t>CustomerNote Table Has DealerID CustomerID and NoteTypeID</t>
+  </si>
+  <si>
+    <t>Landscape Lighting</t>
+  </si>
+  <si>
+    <t>Out: CustomerNote.NoteTypeID='33'</t>
+  </si>
+  <si>
+    <t>CustomerNote.NoteTypeID='33'</t>
+  </si>
+  <si>
+    <t>ChkPetSensitivities</t>
+  </si>
+  <si>
+    <t>CustomerNote.CustomerID  ??</t>
+  </si>
+  <si>
+    <t>TxtSensitivitiesNote</t>
+  </si>
+  <si>
+    <t>CustomerNote.CustomerID ??</t>
+  </si>
+  <si>
+    <t>RB_GPS_PKG</t>
+  </si>
+  <si>
+    <t>Parts.Quantity = 1</t>
+  </si>
+  <si>
+    <t>RB_BPT_PKG</t>
+  </si>
+  <si>
+    <t>RB_DT_PKG</t>
+  </si>
+  <si>
+    <t>GPSPrice</t>
+  </si>
+  <si>
+    <t>ISPrice</t>
+  </si>
+  <si>
+    <t>MSQuantity</t>
+  </si>
+  <si>
+    <t>MSPrice</t>
+  </si>
+  <si>
+    <t>SCQuantity</t>
+  </si>
+  <si>
+    <t>SCPrice</t>
+  </si>
+  <si>
+    <t>MCQuantity</t>
+  </si>
+  <si>
+    <t>Initialize Quantity 0</t>
+  </si>
+  <si>
+    <t>MCPrice</t>
+  </si>
+  <si>
+    <t>DPDQuantity</t>
+  </si>
+  <si>
+    <t>DPDPrice</t>
+  </si>
+  <si>
+    <t>Entered, not predetermined</t>
+  </si>
+  <si>
+    <t>PDF only</t>
+  </si>
+  <si>
+    <t>Email optionally to customer and cc to ccc.invisiblefence.net</t>
+  </si>
+  <si>
+    <t>Note Object</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Part Number or use Discoount part number??</t>
+  </si>
+  <si>
+    <t>Pet Birthdate</t>
   </si>
 </sst>
 </file>
@@ -731,7 +785,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -833,21 +887,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color auto="1"/>
       </left>
@@ -902,12 +941,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -975,16 +1042,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -996,7 +1060,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1005,7 +1069,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1014,23 +1078,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1350,10 +1438,10 @@
   <dimension ref="A1:R80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R79" sqref="R1:R79"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3829,1452 +3917,2338 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E191"/>
+  <dimension ref="A1:M183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C1:C4"/>
+      <selection pane="bottomRight" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="46" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="46" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" style="31" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" style="45" customWidth="1"/>
+    <col min="2" max="2" width="18" style="44" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="45" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="44" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="7" max="11" width="10.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="22.85546875" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E1" s="29" t="s">
+      <c r="D1" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="34" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="52"/>
+      <c r="L2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="47"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B3" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="29"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="39" t="s">
+      <c r="C4" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="30"/>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="E4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="47"/>
+    </row>
+    <row r="5" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="29"/>
+    </row>
+    <row r="7" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="29"/>
+    </row>
+    <row r="8" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="29"/>
+    </row>
+    <row r="9" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="29"/>
+    </row>
+    <row r="10" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="29"/>
+    </row>
+    <row r="11" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="29"/>
+    </row>
+    <row r="12" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="29"/>
+    </row>
+    <row r="13" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="29"/>
+    </row>
+    <row r="14" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="29"/>
+    </row>
+    <row r="15" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="29"/>
+    </row>
+    <row r="16" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="30"/>
-    </row>
-    <row r="4" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="41" t="s">
+      <c r="C16" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="29"/>
+    </row>
+    <row r="17" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="30"/>
-    </row>
-    <row r="6" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="30"/>
-    </row>
-    <row r="7" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="30"/>
-    </row>
-    <row r="9" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="30"/>
-    </row>
-    <row r="10" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="40" t="s">
+      <c r="C17" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="C10" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="30"/>
-    </row>
-    <row r="11" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" s="30"/>
-    </row>
-    <row r="12" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="40" t="s">
+    </row>
+    <row r="18" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="29"/>
+    </row>
+    <row r="19" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>217</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="29"/>
+    </row>
+    <row r="20" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M20" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="C12" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="30"/>
-    </row>
-    <row r="15" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" s="30"/>
-    </row>
-    <row r="16" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="30" t="s">
+    </row>
+    <row r="21" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M21" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M22" s="29" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="2"/>
+      <c r="L23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M23" s="29" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="2"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="29" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="39" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
-        <v>185</v>
-      </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="E19" s="30" t="s">
+      <c r="C25" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="2"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="29" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="39" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="40" t="s">
+      <c r="C26" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="2"/>
+      <c r="L26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="C25" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D25" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="41" t="s">
-        <v>186</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>186</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="40" t="s">
-        <v>190</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>196</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="2"/>
+      <c r="L27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="29"/>
+    </row>
+    <row r="28" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" s="41" t="s">
         <v>191</v>
       </c>
-      <c r="C28" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D28" s="42" t="s">
+      <c r="E28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M28" s="29"/>
+    </row>
+    <row r="29" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="D29" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" s="29"/>
+    </row>
+    <row r="30" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="29"/>
+    </row>
+    <row r="31" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>225</v>
+      </c>
+      <c r="C31" s="40"/>
+      <c r="D31" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="29"/>
+    </row>
+    <row r="32" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" s="29"/>
+    </row>
+    <row r="33" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" s="40"/>
+      <c r="D33" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="29"/>
+    </row>
+    <row r="34" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="2"/>
+      <c r="L34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="29"/>
+    </row>
+    <row r="35" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="C35" s="40"/>
+      <c r="D35" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" s="2"/>
+      <c r="L35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M35" s="29"/>
+    </row>
+    <row r="36" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" s="2"/>
+      <c r="L36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M36" s="29"/>
+    </row>
+    <row r="37" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>232</v>
+      </c>
+      <c r="C37" s="40"/>
+      <c r="D37" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" s="2"/>
+      <c r="L37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37" s="29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" s="2"/>
+      <c r="L38" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="2"/>
+      <c r="L39" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" s="29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D40" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="4"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K40" s="2"/>
+      <c r="L40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M40" s="29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="39"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M41" s="29"/>
+    </row>
+    <row r="42" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" s="42"/>
+      <c r="C42" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D42" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K42" s="2"/>
+      <c r="L42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M42" s="29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="42"/>
+      <c r="C43" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="4"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K43" s="2"/>
+      <c r="L43" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M43" s="29"/>
+    </row>
+    <row r="44" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="42"/>
+      <c r="C44" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D44" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44" s="2"/>
+      <c r="L44" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M44" s="29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="42"/>
+      <c r="C45" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D45" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="4"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="2"/>
+      <c r="L45" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M45" s="29"/>
+    </row>
+    <row r="46" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B46" s="42"/>
+      <c r="C46" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D46" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="4"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" s="2"/>
+      <c r="L46" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M46" s="29"/>
+    </row>
+    <row r="47" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="42"/>
+      <c r="C47" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D47" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K47" s="2"/>
+      <c r="L47" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M47" s="29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="42"/>
+      <c r="C48" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D48" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K48" s="2"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="29"/>
+    </row>
+    <row r="49" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="42"/>
+      <c r="C49" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D49" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K49" s="2"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="29"/>
+    </row>
+    <row r="50" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" s="42"/>
+      <c r="C50" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K50" s="2"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" s="42"/>
+      <c r="C51" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D51" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K51" s="2"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="29"/>
+    </row>
+    <row r="52" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" s="42"/>
+      <c r="C52" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D52" s="43"/>
+      <c r="E52" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K52" s="2"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" s="42"/>
+      <c r="C53" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D53" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G53" s="4"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K53" s="2"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="29"/>
+    </row>
+    <row r="54" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="42"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K54" s="2"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" s="42"/>
+      <c r="C55" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="D55" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="42" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" s="42"/>
+      <c r="C56" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="D56" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K56" s="2"/>
+      <c r="L56" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M56" s="29"/>
+    </row>
+    <row r="57" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" s="42"/>
+      <c r="C57" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="D57" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="29" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" s="42"/>
+      <c r="C58" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="D58" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K58" s="2"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" s="42"/>
+      <c r="C59" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="D59" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K59" s="2"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="29" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" s="42"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" s="42"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="42"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" s="28" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="B63" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="C63" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="29"/>
+    </row>
+    <row r="64" spans="1:13" s="28" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="B64" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="C64" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D64" s="43"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K64" s="2"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="B65" s="42"/>
+      <c r="C65" s="29" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="41" t="s">
-        <v>186</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>186</v>
-      </c>
-      <c r="E29" s="30" t="s">
+      <c r="D65" s="43"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="29" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" s="28" customFormat="1" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="B66" s="42"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="54"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="29" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" s="28" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="B67" s="42"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="44"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="29" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="B68" s="42"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="43"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="29"/>
+    </row>
+    <row r="69" spans="1:13" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="B69" s="42"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" s="28" customFormat="1" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="B70" s="42"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="43" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>196</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E30" s="30"/>
-    </row>
-    <row r="31" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E31" s="30"/>
-    </row>
-    <row r="32" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="30"/>
-    </row>
-    <row r="33" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E33" s="30"/>
-    </row>
-    <row r="34" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E34" s="30"/>
-    </row>
-    <row r="35" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="30"/>
-    </row>
-    <row r="36" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E36" s="30"/>
-    </row>
-    <row r="37" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D37" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E37" s="30"/>
-    </row>
-    <row r="38" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="40"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="30"/>
-    </row>
-    <row r="39" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="40"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E39" s="30"/>
-    </row>
-    <row r="40" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D40" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E40" s="30"/>
-    </row>
-    <row r="41" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="30"/>
-    </row>
-    <row r="42" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E42" s="30"/>
-    </row>
-    <row r="43" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="40"/>
-      <c r="C43" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D43" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E43" s="30"/>
-    </row>
-    <row r="44" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B44" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" s="41"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="D45" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D46" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E46" s="30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="40"/>
-      <c r="C47" s="41" t="s">
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L70" s="4"/>
+      <c r="M70" s="29"/>
+    </row>
+    <row r="71" spans="1:13" s="28" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" s="42"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L71" s="4"/>
+      <c r="M71" s="29"/>
+    </row>
+    <row r="72" spans="1:13" s="28" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B72" s="42"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="D48" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E48" s="30"/>
-    </row>
-    <row r="49" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="B49" s="43"/>
-      <c r="C49" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D49" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E49" s="30"/>
-    </row>
-    <row r="50" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="B50" s="43"/>
-      <c r="C50" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="D50" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E50" s="30"/>
-    </row>
-    <row r="51" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D51" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E51" s="30"/>
-    </row>
-    <row r="52" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="B52" s="43"/>
-      <c r="C52" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="D52" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="E52" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="D53" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="E53" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="B54" s="43"/>
-      <c r="C54" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D54" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E54" s="30"/>
-    </row>
-    <row r="55" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="B55" s="43"/>
-      <c r="C55" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="D55" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E55" s="30"/>
-    </row>
-    <row r="56" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="B56" s="43"/>
-      <c r="C56" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D56" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E56" s="30"/>
-    </row>
-    <row r="57" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="B57" s="43"/>
-      <c r="C57" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D57" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E57" s="30"/>
-    </row>
-    <row r="58" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="B58" s="43"/>
-      <c r="C58" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="D58" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E58" s="30"/>
-    </row>
-    <row r="59" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="B59" s="43"/>
-      <c r="C59" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D59" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E59" s="30"/>
-    </row>
-    <row r="60" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="B60" s="43"/>
-      <c r="C60" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="D60" s="44"/>
-      <c r="E60" s="30"/>
-    </row>
-    <row r="61" spans="1:5" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="B61" s="43"/>
-      <c r="C61" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D61" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E61" s="30"/>
-    </row>
-    <row r="62" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="B62" s="43"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="44"/>
-      <c r="E62" s="30"/>
-    </row>
-    <row r="63" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="B63" s="43"/>
-      <c r="C63" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="D63" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="E63" s="30" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="42" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="B64" s="43"/>
-      <c r="C64" s="30" t="s">
-        <v>218</v>
-      </c>
-      <c r="D64" s="42" t="s">
-        <v>205</v>
-      </c>
-      <c r="E64" s="30"/>
-    </row>
-    <row r="65" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="B65" s="43"/>
-      <c r="C65" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="D65" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="E65" s="30" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="B66" s="43"/>
-      <c r="C66" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="D66" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="E66" s="30" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="B67" s="43"/>
-      <c r="C67" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="D67" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="E67" s="30"/>
-    </row>
-    <row r="68" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="B68" s="43"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="44"/>
-      <c r="E68" s="30" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="45" t="s">
-        <v>125</v>
-      </c>
-      <c r="B69" s="43"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="44"/>
-      <c r="E69" s="30" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="B70" s="43"/>
-      <c r="C70" s="30"/>
-      <c r="D70" s="44"/>
-      <c r="E70" s="30" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="28" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="45" t="s">
-        <v>151</v>
-      </c>
-      <c r="B71" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="C71" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="D71" s="44" t="s">
-        <v>152</v>
-      </c>
-      <c r="E71" s="30"/>
-    </row>
-    <row r="72" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="45" t="s">
-        <v>209</v>
-      </c>
-      <c r="B72" s="43" t="s">
-        <v>210</v>
-      </c>
-      <c r="C72" s="30" t="s">
-        <v>211</v>
-      </c>
-      <c r="D72" s="44"/>
-      <c r="E72" s="30" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="B73" s="43"/>
-      <c r="C73" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="D73" s="44"/>
-      <c r="E73" s="30" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="28" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="B74" s="43"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="30" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B75" s="43"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="46"/>
-      <c r="E75" s="30" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="B76" s="43"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="44"/>
-      <c r="E76" s="30"/>
-    </row>
-    <row r="77" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="45" t="s">
-        <v>160</v>
-      </c>
-      <c r="B77" s="43"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="46"/>
-      <c r="E77" s="30" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="28" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="45" t="s">
-        <v>162</v>
-      </c>
-      <c r="B78" s="43"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="44" t="s">
-        <v>215</v>
-      </c>
-      <c r="E78" s="30"/>
-    </row>
-    <row r="79" spans="1:5" s="28" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="B79" s="43"/>
-      <c r="C79" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="D79" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="E79" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="28" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="B80" s="43"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="E80" s="30"/>
-    </row>
-    <row r="81" spans="5:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E81" s="32"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="33"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="33"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="33"/>
-    </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E85" s="33"/>
-    </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E86" s="33"/>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E87" s="33"/>
-    </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E88" s="33"/>
-    </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E89" s="33"/>
-    </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E90" s="33"/>
-    </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E91" s="33"/>
-    </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E92" s="33"/>
-    </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E93" s="33"/>
-    </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E94" s="33"/>
-    </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E95" s="33"/>
-    </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E96" s="33"/>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E97" s="33"/>
-    </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E98" s="33"/>
-    </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E99" s="33"/>
-    </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E100" s="33"/>
-    </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E101" s="33"/>
-    </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E102" s="33"/>
-    </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E103" s="33"/>
-    </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E104" s="33"/>
-    </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E105" s="33"/>
-    </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E106" s="33"/>
-    </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E107" s="33"/>
-    </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E108" s="33"/>
-    </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E109" s="33"/>
-    </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E110" s="33"/>
-    </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E111" s="33"/>
-    </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E112" s="33"/>
-    </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E113" s="33"/>
-    </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E114" s="33"/>
-    </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E115" s="33"/>
-    </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E116" s="33"/>
-    </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E117" s="33"/>
-    </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E118" s="33"/>
-    </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E119" s="33"/>
-    </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E120" s="33"/>
-    </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E121" s="33"/>
-    </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E122" s="33"/>
-    </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E123" s="33"/>
-    </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E124" s="33"/>
-    </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E125" s="33"/>
-    </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E126" s="33"/>
-    </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E127" s="33"/>
-    </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E128" s="33"/>
-    </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E129" s="33"/>
-    </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E130" s="33"/>
-    </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E131" s="33"/>
-    </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E132" s="33"/>
-    </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E133" s="33"/>
-    </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E134" s="33"/>
-    </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E135" s="33"/>
-    </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E136" s="33"/>
-    </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E137" s="33"/>
-    </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E138" s="33"/>
-    </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E139" s="33"/>
-    </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E140" s="33"/>
-    </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E141" s="33"/>
-    </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E142" s="33"/>
-    </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E143" s="33"/>
-    </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E144" s="33"/>
-    </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E145" s="33"/>
-    </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E146" s="33"/>
-    </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E147" s="33"/>
-    </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E148" s="33"/>
-    </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E149" s="33"/>
-    </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E150" s="33"/>
-    </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E151" s="33"/>
-    </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E152" s="33"/>
-    </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E153" s="33"/>
-    </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E154" s="33"/>
-    </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E155" s="33"/>
-    </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E156" s="33"/>
-    </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E157" s="33"/>
-    </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E158" s="33"/>
-    </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E159" s="33"/>
-    </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E160" s="33"/>
-    </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E161" s="33"/>
-    </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E162" s="33"/>
-    </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E163" s="33"/>
-    </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E164" s="33"/>
-    </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E165" s="33"/>
-    </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E166" s="33"/>
-    </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E167" s="33"/>
-    </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E168" s="33"/>
-    </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E169" s="33"/>
-    </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E170" s="33"/>
-    </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E171" s="33"/>
-    </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E172" s="33"/>
-    </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E173" s="33"/>
-    </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E174" s="33"/>
-    </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E175" s="33"/>
-    </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E176" s="33"/>
-    </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E177" s="33"/>
-    </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E178" s="33"/>
-    </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E179" s="33"/>
-    </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E180" s="33"/>
-    </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E181" s="33"/>
-    </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E182" s="33"/>
-    </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E183" s="33"/>
-    </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E184" s="33"/>
-    </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E185" s="33"/>
-    </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E186" s="33"/>
-    </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E187" s="33"/>
-    </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E188" s="33"/>
-    </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E189" s="33"/>
-    </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E190" s="33"/>
-    </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E191" s="33"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="29" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M73" s="31"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M74" s="32"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M75" s="32"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M76" s="32"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M77" s="32"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M78" s="32"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M79" s="32"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M80" s="32"/>
+    </row>
+    <row r="81" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M81" s="32"/>
+    </row>
+    <row r="82" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M82" s="32"/>
+    </row>
+    <row r="83" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M83" s="32"/>
+    </row>
+    <row r="84" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M84" s="32"/>
+    </row>
+    <row r="85" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M85" s="32"/>
+    </row>
+    <row r="86" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M86" s="32"/>
+    </row>
+    <row r="87" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M87" s="32"/>
+    </row>
+    <row r="88" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M88" s="32"/>
+    </row>
+    <row r="89" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M89" s="32"/>
+    </row>
+    <row r="90" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M90" s="32"/>
+    </row>
+    <row r="91" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M91" s="32"/>
+    </row>
+    <row r="92" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M92" s="32"/>
+    </row>
+    <row r="93" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M93" s="32"/>
+    </row>
+    <row r="94" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M94" s="32"/>
+    </row>
+    <row r="95" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M95" s="32"/>
+    </row>
+    <row r="96" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M96" s="32"/>
+    </row>
+    <row r="97" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M97" s="32"/>
+    </row>
+    <row r="98" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M98" s="32"/>
+    </row>
+    <row r="99" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M99" s="32"/>
+    </row>
+    <row r="100" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M100" s="32"/>
+    </row>
+    <row r="101" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M101" s="32"/>
+    </row>
+    <row r="102" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M102" s="32"/>
+    </row>
+    <row r="103" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M103" s="32"/>
+    </row>
+    <row r="104" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M104" s="32"/>
+    </row>
+    <row r="105" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M105" s="32"/>
+    </row>
+    <row r="106" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M106" s="32"/>
+    </row>
+    <row r="107" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M107" s="32"/>
+    </row>
+    <row r="108" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M108" s="32"/>
+    </row>
+    <row r="109" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M109" s="32"/>
+    </row>
+    <row r="110" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M110" s="32"/>
+    </row>
+    <row r="111" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M111" s="32"/>
+    </row>
+    <row r="112" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M112" s="32"/>
+    </row>
+    <row r="113" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M113" s="32"/>
+    </row>
+    <row r="114" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M114" s="32"/>
+    </row>
+    <row r="115" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M115" s="32"/>
+    </row>
+    <row r="116" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M116" s="32"/>
+    </row>
+    <row r="117" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M117" s="32"/>
+    </row>
+    <row r="118" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M118" s="32"/>
+    </row>
+    <row r="119" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M119" s="32"/>
+    </row>
+    <row r="120" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M120" s="32"/>
+    </row>
+    <row r="121" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M121" s="32"/>
+    </row>
+    <row r="122" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M122" s="32"/>
+    </row>
+    <row r="123" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M123" s="32"/>
+    </row>
+    <row r="124" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M124" s="32"/>
+    </row>
+    <row r="125" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M125" s="32"/>
+    </row>
+    <row r="126" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M126" s="32"/>
+    </row>
+    <row r="127" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M127" s="32"/>
+    </row>
+    <row r="128" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M128" s="32"/>
+    </row>
+    <row r="129" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M129" s="32"/>
+    </row>
+    <row r="130" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M130" s="32"/>
+    </row>
+    <row r="131" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M131" s="32"/>
+    </row>
+    <row r="132" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M132" s="32"/>
+    </row>
+    <row r="133" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M133" s="32"/>
+    </row>
+    <row r="134" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M134" s="32"/>
+    </row>
+    <row r="135" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M135" s="32"/>
+    </row>
+    <row r="136" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M136" s="32"/>
+    </row>
+    <row r="137" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M137" s="32"/>
+    </row>
+    <row r="138" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M138" s="32"/>
+    </row>
+    <row r="139" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M139" s="32"/>
+    </row>
+    <row r="140" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M140" s="32"/>
+    </row>
+    <row r="141" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M141" s="32"/>
+    </row>
+    <row r="142" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M142" s="32"/>
+    </row>
+    <row r="143" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M143" s="32"/>
+    </row>
+    <row r="144" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M144" s="32"/>
+    </row>
+    <row r="145" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M145" s="32"/>
+    </row>
+    <row r="146" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M146" s="32"/>
+    </row>
+    <row r="147" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M147" s="32"/>
+    </row>
+    <row r="148" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M148" s="32"/>
+    </row>
+    <row r="149" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M149" s="32"/>
+    </row>
+    <row r="150" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M150" s="32"/>
+    </row>
+    <row r="151" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M151" s="32"/>
+    </row>
+    <row r="152" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M152" s="32"/>
+    </row>
+    <row r="153" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M153" s="32"/>
+    </row>
+    <row r="154" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M154" s="32"/>
+    </row>
+    <row r="155" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M155" s="32"/>
+    </row>
+    <row r="156" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M156" s="32"/>
+    </row>
+    <row r="157" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M157" s="32"/>
+    </row>
+    <row r="158" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M158" s="32"/>
+    </row>
+    <row r="159" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M159" s="32"/>
+    </row>
+    <row r="160" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M160" s="32"/>
+    </row>
+    <row r="161" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M161" s="32"/>
+    </row>
+    <row r="162" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M162" s="32"/>
+    </row>
+    <row r="163" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M163" s="32"/>
+    </row>
+    <row r="164" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M164" s="32"/>
+    </row>
+    <row r="165" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M165" s="32"/>
+    </row>
+    <row r="166" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M166" s="32"/>
+    </row>
+    <row r="167" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M167" s="32"/>
+    </row>
+    <row r="168" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M168" s="32"/>
+    </row>
+    <row r="169" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M169" s="32"/>
+    </row>
+    <row r="170" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M170" s="32"/>
+    </row>
+    <row r="171" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M171" s="32"/>
+    </row>
+    <row r="172" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M172" s="32"/>
+    </row>
+    <row r="173" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M173" s="32"/>
+    </row>
+    <row r="174" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M174" s="32"/>
+    </row>
+    <row r="175" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M175" s="32"/>
+    </row>
+    <row r="176" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M176" s="32"/>
+    </row>
+    <row r="177" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M177" s="32"/>
+    </row>
+    <row r="178" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M178" s="32"/>
+    </row>
+    <row r="179" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M179" s="32"/>
+    </row>
+    <row r="180" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M180" s="32"/>
+    </row>
+    <row r="181" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M181" s="32"/>
+    </row>
+    <row r="182" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M182" s="32"/>
+    </row>
+    <row r="183" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M183" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>